<commit_message>
test s6-1 on model gpt3.5
</commit_message>
<xml_diff>
--- a/json/bug_gpt_json/raw/s6-1.xlsx
+++ b/json/bug_gpt_json/raw/s6-1.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20338"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\project2\ANT\ChatGptStudy\json\bug_gpt_json\raw\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\学习资料\学校课程\研究生\项目\陈厅\蚂蚁\ChatGptStudy\json\bug_gpt_json\raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED7DAAC3-3BBF-4828-9153-CFC099368818}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1875" yWindow="0" windowWidth="20850" windowHeight="12090" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2808" yWindow="0" windowWidth="20856" windowHeight="12096"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="805" uniqueCount="803">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="845" uniqueCount="843">
   <si>
     <t>vul</t>
   </si>
@@ -12087,11 +12086,688 @@
   <si>
     <t>A vulnerability arises due to incorrect calculation order when updating token balances and prices.</t>
   </si>
+  <si>
+    <t xml:space="preserve">// SPDX-License-Identifier: MIT
+pragma solidity ^0.8.0;
+contract EthLoan {
+    struct Loan {
+        uint256 amount;
+        uint256 startBlock;
+    }
+    uint256 public interestRatePerBlock = 1;  // 0.01% per block as an example
+    mapping(address =&gt; Loan) public loans;
+    event LoanTaken(address indexed user, uint256 amount);
+    function takeLoan(uint256 amount) external payable {
+        require(msg.value == amount, "Amount mismatch!");
+        // Vulnerability: Calculate and update interest before setting the new start block
+        if (loans[msg.sender].amount != 0) {
+            uint256 interest = (block.number - loans[msg.sender].startBlock) * interestRatePerBlock * loans[msg.sender].amount / 10000;
+            loans[msg.sender].amount += interest;
+        }
+        loans[msg.sender].amount += amount;
+        loans[msg.sender].startBlock = block.number;
+        emit LoanTaken(msg.sender, amount);
+    }
+    function repayLoan() external payable {
+        require(loans[msg.sender].amount &gt; 0, "No loan taken.");
+        uint256 totalDue = loans[msg.sender].amount + (block.number - loans[msg.sender].startBlock) * interestRatePerBlock * loans[msg.sender].amount / 10000;
+        require(msg.value &gt;= totalDue, "Not enough to cover the loan and interest.");
+        payable(msg.sender).transfer(msg.value - totalDue);  // Refund any excess
+        delete loans[msg.sender];  // Clear the loan
+    }
+}
+</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">// SPDX-License-Identifier: MIT
+pragma solidity ^0.8.0;
+contract EthLoan {
+    struct Loan {
+        uint256 amount;
+        uint256 startBlock;
+    }
+    uint256 public interestRatePerBlock = 1;  // 0.01% per block as an example
+    mapping(address =&gt; Loan) public loans;
+    event LoanTaken(address indexed user, uint256 amount);
+    function takeLoan(uint256 amount) external payable {
+        require(msg.value == amount, "Amount mismatch!");
+        // Fix: Update start block first to avoid malicious exploitation of the interest calculation
+        uint256 oldStartBlock = loans[msg.sender].startBlock;
+        loans[msg.sender].startBlock = block.number;
+        if (loans[msg.sender].amount != 0) {
+            uint256 interest = (block.number - oldStartBlock) * interestRatePerBlock * loans[msg.sender].amount / 10000;
+            loans[msg.sender].amount += interest;
+        }
+        loans[msg.sender].amount += amount;
+        emit LoanTaken(msg.sender, amount);
+    }
+    function repayLoan() external payable {
+        require(loans[msg.sender].amount &gt; 0, "No loan taken.");
+        uint256 totalDue = loans[msg.sender].amount + (block.number - loans[msg.sender].startBlock) * interestRatePerBlock * loans[msg.sender].amount / 10000;
+        require(msg.value &gt;= totalDue, "Not enough to cover the loan and interest.");
+        payable(msg.sender).transfer(msg.value - totalDue);  // Refund any excess
+        delete loans[msg.sender];  // Clear the loan
+    }
+}
+</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">if (loans[msg.sender].amount != 0) {
+            uint256 interest = (block.number - loans[msg.sender].startBlock) * interestRatePerBlock * loans[msg.sender].amount / 10000;
+            loans[msg.sender].amount += interest;
+        }
+        loans[msg.sender].amount += amount;
+        loans[msg.sender].startBlock = block.number;
+</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>A contract allows users to deposit Ethereum and rewards them with a token. The number of tokens they receive is calculated based on the current token price. However, there's a vulnerability due to the incorrect order of updating the total deposit balance and the current token price.</t>
+  </si>
+  <si>
+    <t>A contract allows users to loan Ethereum, receiving interest over time. The interest is calculated based on the number of blocks since the loan was taken. A vulnerability arises due to the incorrect order in which the interest calculation and user balance update occur.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">// SPDX-License-Identifier: MIT
+pragma solidity ^0.8.0;
+contract EthDepositReward {
+    uint256 public totalDeposits;
+    uint256 public tokenPrice = 1 ether;  // Starting token price as 1 ETH for simplicity.
+    mapping(address =&gt; uint256) public balances;
+    mapping(address =&gt; uint256) public rewards;
+    event Deposited(address indexed user, uint256 amount, uint256 rewardAmount);
+    function deposit() external payable {
+        require(msg.value &gt; 0, "Deposit value should be greater than 0");
+        // Vulnerability: Updating token price before calculating the reward.
+        tokenPrice = totalDeposits / 1000;  // Example: The more total deposits, the lesser the token price.
+        uint256 rewardAmount = msg.value / tokenPrice;
+        balances[msg.sender] += msg.value;
+        totalDeposits += msg.value;
+        rewards[msg.sender] += rewardAmount;
+        emit Deposited(msg.sender, msg.value, rewardAmount);
+    }
+    // Additional functions would be here...
+}
+</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">// SPDX-License-Identifier: MIT
+pragma solidity ^0.8.0;
+contract EthDepositReward {
+    uint256 public totalDeposits;
+    uint256 public tokenPrice = 1 ether;  // Starting token price as 1 ETH for simplicity.
+    mapping(address =&gt; uint256) public balances;
+    mapping(address =&gt; uint256) public rewards;
+    event Deposited(address indexed user, uint256 amount, uint256 rewardAmount);
+    function deposit() external payable {
+        require(msg.value &gt; 0, "Deposit value should be greater than 0");
+        // Fix: Update totalDeposits first before recalculating token price.
+        totalDeposits += msg.value;
+        tokenPrice = totalDeposits / 1000;  // Example: The more total deposits, the lesser the token price.
+        uint256 rewardAmount = msg.value / tokenPrice;
+        balances[msg.sender] += msg.value;
+        rewards[msg.sender] += rewardAmount;
+        emit Deposited(msg.sender, msg.value, rewardAmount);
+    }
+    // Additional functions would be here...
+}
+</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>tokenPrice = totalDeposits / 1000;  // Example: The more total deposits, the lesser the token price.
+        uint256 rewardAmount = msg.value / tokenPrice;
+        balances[msg.sender] += msg.value;
+        totalDeposits += msg.value;
+        rewards[msg.sender] += rewardAmount;</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>In a simple staking contract, users can stake tokens and after a certain time, they can claim their rewards which are calculated based on the total time staked. However, there is a vulnerability in the claimReward function due to the incorrect order of updating the user's last claim time and calculating the reward.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">// SPDX-License-Identifier: MIT
+pragma solidity ^0.8.0;
+contract SimpleStaking {
+    uint256 public rewardRate = 1e18;  // For simplicity, let's say 1 token reward per second.
+    struct User {
+        uint256 balance;
+        uint256 lastClaimTime;
+    }
+    mapping(address =&gt; User) public users;
+    event RewardClaimed(address indexed user, uint256 amount);
+    function stake(uint256 amount) external {
+        // Assume a transfer function exists that moves tokens into the contract
+        // For simplicity, it's omitted here.
+        User storage user = users[msg.sender];
+        user.balance += amount;
+        user.lastClaimTime = block.timestamp;
+    }
+    function claimReward() external {
+        User storage user = users[msg.sender];
+        // Vulnerability: Updating lastClaimTime before calculating the reward.
+        uint256 timeElapsed = block.timestamp - user.lastClaimTime;
+        user.lastClaimTime = block.timestamp;
+        uint256 reward = timeElapsed * rewardRate;
+        require(reward &lt;= user.balance, "Not enough tokens to give as reward");
+        // Simulate the transfer of reward to the user
+        user.balance -= reward;
+        emit RewardClaimed(msg.sender, reward);
+    }
+    // Additional functions would be here...
+}
+</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>uint256 timeElapsed = block.timestamp - user.lastClaimTime;
+        user.lastClaimTime = block.timestamp;
+        uint256 reward = timeElapsed * rewardRate;
+        require(reward &lt;= user.balance, "Not enough tokens to give as reward");
+        // Simulate the transfer of reward to the user
+        user.balance -= reward;</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">// SPDX-License-Identifier: MIT
+pragma solidity ^0.8.0;
+contract SimpleStaking {
+    uint256 public rewardRate = 1e18;  // For simplicity, let's say 1 token reward per second.
+    struct User {
+        uint256 balance;
+        uint256 lastClaimTime;
+    }
+    mapping(address =&gt; User) public users;
+    event RewardClaimed(address indexed user, uint256 amount);
+    function stake(uint256 amount) external {
+        // Assume a transfer function exists that moves tokens into the contract
+        // For simplicity, it's omitted here.
+        User storage user = users[msg.sender];
+        user.balance += amount;
+        user.lastClaimTime = block.timestamp;
+    }
+    function claimReward() external {
+        User storage user = users[msg.sender];
+        // Fix: Calculate the reward before updating the lastClaimTime.
+        uint256 timeElapsed = block.timestamp - user.lastClaimTime;
+        uint256 reward = timeElapsed * rewardRate;
+        user.lastClaimTime = block.timestamp;
+        require(reward &lt;= user.balance, "Not enough tokens to give as reward");
+        // Simulate the transfer of reward to the user
+        user.balance -= reward;
+        emit RewardClaimed(msg.sender, reward);
+    }
+    // Additional functions would be here...
+}
+</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>A savings contract allows users to deposit tokens. The interest is calculated based on the total time the tokens have been held. The flaw is in the withdraw function, which calculates interest before updating the user's last deposit time, allowing users to potentially exploit the contract by frequently withdrawing and depositing.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">// SPDX-License-Identifier: MIT
+pragma solidity ^0.8.0;
+contract SimpleSavings {
+    uint256 public interestRate = 1e15;  // Representing 0.1% interest per second for simplicity.
+    struct Account {
+        uint256 balance;
+        uint256 lastDepositTime;
+    }
+    mapping(address =&gt; Account) public accounts;
+    event Withdrawn(address indexed user, uint256 amount);
+    function deposit(uint256 amount) external {
+        // Assume a function that transfers tokens into the contract exists.
+        // Omitted for brevity.
+        Account storage userAccount = accounts[msg.sender];
+        userAccount.balance += amount;
+        userAccount.lastDepositTime = block.timestamp;
+    }
+    function withdraw(uint256 amount) external {
+        Account storage userAccount = accounts[msg.sender];
+        // Vulnerability: Calculating interest before updating the lastDepositTime.
+        uint256 timeElapsed = block.timestamp - userAccount.lastDepositTime;
+        uint256 interest = userAccount.balance * interestRate * timeElapsed;
+        userAccount.lastDepositTime = block.timestamp;
+        uint256 totalWithdrawal = amount + interest;
+        require(totalWithdrawal &lt;= userAccount.balance, "Insufficient balance");
+        // Simulate the transfer of the withdrawal amount to the user.
+        userAccount.balance -= totalWithdrawal;
+        emit Withdrawn(msg.sender, totalWithdrawal);
+    }
+    // ... other functions.
+}
+</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">// SPDX-License-Identifier: MIT
+pragma solidity ^0.8.0;
+contract SimpleSavings {
+    uint256 public interestRate = 1e15;  // Representing 0.1% interest per second for simplicity.
+    struct Account {
+        uint256 balance;
+        uint256 lastDepositTime;
+    }
+    mapping(address =&gt; Account) public accounts;
+    event Withdrawn(address indexed user, uint256 amount);
+    function deposit(uint256 amount) external {
+        // Assume a function that transfers tokens into the contract exists.
+        // Omitted for brevity.
+        Account storage userAccount = accounts[msg.sender];
+        userAccount.balance += amount;
+        userAccount.lastDepositTime = block.timestamp;
+    }
+    function withdraw(uint256 amount) external {
+        Account storage userAccount = accounts[msg.sender];
+        // Fix: Update the lastDepositTime before calculating the interest.
+        uint256 timeElapsed = block.timestamp - userAccount.lastDepositTime;
+        userAccount.lastDepositTime = block.timestamp;
+        uint256 interest = userAccount.balance * interestRate * timeElapsed;
+        uint256 totalWithdrawal = amount + interest;
+        require(totalWithdrawal &lt;= userAccount.balance, "Insufficient balance");
+        // Simulate the transfer of the withdrawal amount to the user.
+        userAccount.balance -= totalWithdrawal;
+        emit Withdrawn(msg.sender, totalWithdrawal);
+    }
+    // ... other functions.
+}
+</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>uint256 timeElapsed = block.timestamp - userAccount.lastDepositTime;
+        uint256 interest = userAccount.balance * interestRate * timeElapsed;
+        userAccount.lastDepositTime = block.timestamp;
+        uint256 totalWithdrawal = amount + interest;
+        require(totalWithdrawal &lt;= userAccount.balance, "Insufficient balance");
+        // Simulate the transfer of the withdrawal amount to the user.
+        userAccount.balance -= totalWithdrawal;</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>The contract flaw is in the buyTicket function: the contract checks if the event has enough tickets after it decrements the number of available tickets, allowing users to potentially purchase more tickets than available.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">// SPDX-License-Identifier: MIT
+pragma solidity ^0.8.0;
+contract EventTickets {
+    struct Event {
+        string name;
+        uint256 ticketPrice;
+        uint256 totalTickets;
+        uint256 ticketsSold;
+    }
+    mapping(uint256 =&gt; Event) public events;
+    uint256 public nextEventId = 0;
+    event TicketPurchased(uint256 eventId, address buyer, uint256 amount);
+    function createEvent(string calldata _name, uint256 _ticketPrice, uint256 _totalTickets) external {
+        events[nextEventId] = Event({
+            name: _name,
+            ticketPrice: _ticketPrice,
+            totalTickets: _totalTickets,
+            ticketsSold: 0
+        });
+        nextEventId++;
+    }
+    function buyTicket(uint256 _eventId, uint256 _amount) external payable {
+        Event storage chosenEvent = events[_eventId];
+        // Assuming we can do ERC20 transfers or similar. Here we just use ether for simplicity.
+        require(msg.value == chosenEvent.ticketPrice * _amount, "Incorrect Ether sent");
+        // Vulnerability: Decreasing tickets before checking availability.
+        chosenEvent.ticketsSold += _amount;
+        require(chosenEvent.ticketsSold &lt;= chosenEvent.totalTickets, "Not enough tickets available");
+        emit TicketPurchased(_eventId, msg.sender, _amount);
+    }
+    // ... other functions for refunding, event management etc.
+}
+</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">require(msg.value == chosenEvent.ticketPrice * _amount, "Incorrect Ether sent");
+        // Vulnerability: Decreasing tickets before checking availability.
+        chosenEvent.ticketsSold += _amount;
+        require(chosenEvent.ticketsSold &lt;= chosenEvent.totalTickets, "Not enough tickets available");
+</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">// SPDX-License-Identifier: MIT
+pragma solidity ^0.8.0;
+contract EventTickets {
+    struct Event {
+        string name;
+        uint256 ticketPrice;
+        uint256 totalTickets;
+        uint256 ticketsSold;
+    }
+    mapping(uint256 =&gt; Event) public events;
+    uint256 public nextEventId = 0;
+    event TicketPurchased(uint256 eventId, address buyer, uint256 amount);
+    function createEvent(string calldata _name, uint256 _ticketPrice, uint256 _totalTickets) external {
+        events[nextEventId] = Event({
+            name: _name,
+            ticketPrice: _ticketPrice,
+            totalTickets: _totalTickets,
+            ticketsSold: 0
+        });
+        nextEventId++;
+    }
+    function buyTicket(uint256 _eventId, uint256 _amount) external payable {
+        Event storage chosenEvent = events[_eventId];
+        // Assuming we can do ERC20 transfers or similar. Here we just use ether for simplicity.
+        require(msg.value == chosenEvent.ticketPrice * _amount, "Incorrect Ether sent");
+        // Fix: Check ticket availability before updating the ticketsSold.
+        require(chosenEvent.ticketsSold + _amount &lt;= chosenEvent.totalTickets, "Not enough tickets available");
+        chosenEvent.ticketsSold += _amount;
+        emit TicketPurchased(_eventId, msg.sender, _amount);
+    }
+    // ... other functions for refunding, event management etc.
+}
+</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve"> The contract flaw is in the withdraw function: the contract sends the funds to the user before decrementing the user's balance, making it vulnerable to a reentrancy attack.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">// SPDX-License-Identifier: MIT
+pragma solidity ^0.8.0;
+contract VulnerableWallet {
+    mapping(address =&gt; uint256) public balances;
+    event Deposited(address indexed user, uint256 amount);
+    event Withdrawn(address indexed user, uint256 amount);
+    function deposit() external payable {
+        balances[msg.sender] += msg.value;
+        emit Deposited(msg.sender, msg.value);
+    }
+    function withdraw(uint256 _amount) external {
+        require(balances[msg.sender] &gt;= _amount, "Insufficient balance!");
+        // Vulnerability: Sending ether before updating the balance
+        (bool success, ) = msg.sender.call{value: _amount}("");
+        require(success, "Transfer failed!");
+        balances[msg.sender] -= _amount;
+        emit Withdrawn(msg.sender, _amount);
+    }
+    // ... other potential functions
+}
+</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>(bool success, ) = msg.sender.call{value: _amount}("");
+        require(success, "Transfer failed!");
+        balances[msg.sender] -= _amount;</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">// SPDX-License-Identifier: MIT
+pragma solidity ^0.8.0;
+contract SecureWallet {
+    mapping(address =&gt; uint256) public balances;
+    event Deposited(address indexed user, uint256 amount);
+    event Withdrawn(address indexed user, uint256 amount);
+    function deposit() external payable {
+        balances[msg.sender] += msg.value;
+        emit Deposited(msg.sender, msg.value);
+    }
+    function withdraw(uint256 _amount) external {
+        require(balances[msg.sender] &gt;= _amount, "Insufficient balance!");
+        // Fix: Decrease the balance before sending the ether
+        balances[msg.sender] -= _amount;
+        (bool success, ) = msg.sender.call{value: _amount}("");
+        require(success, "Transfer failed!");
+        emit Withdrawn(msg.sender, _amount);
+    }
+    // ... other potential functions
+}
+</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>he vulnerability arises from updating the state of the highest bid after refunding the previous highest bidder. This could allow potential reentrancy attacks.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">// SPDX-License-Identifier: MIT
+pragma solidity ^0.8.0;
+contract VulnerableAuction {
+    address public highestBidder;
+    uint256 public highestBid;
+    event HighestBidIncreased(address indexed bidder, uint256 amount);
+    function bid() external payable {
+        require(msg.value &gt; highestBid, "There's already a higher bid.");
+        // Vulnerability: Refunding before updating the state
+        if (highestBidder != address(0)) {
+            (bool success, ) = highestBidder.call{value: highestBid}("");
+            require(success, "Failed to send back the ether!");
+        }
+        highestBidder = msg.sender;
+        highestBid = msg.value;
+        emit HighestBidIncreased(msg.sender, msg.value);
+    }
+    // ... other functions like auction end, withdrawal, etc.
+}
+</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">// SPDX-License-Identifier: MIT
+pragma solidity ^0.8.0;
+contract SecureAuction {
+    address public highestBidder;
+    uint256 public highestBid;
+    event HighestBidIncreased(address indexed bidder, uint256 amount);
+    function bid() external payable {
+        require(msg.value &gt; highestBid, "There's already a higher bid.");
+        address previousHighestBidder = highestBidder;
+        uint256 refundAmount = highestBid;
+        // Fix: Update the state before any transfer
+        highestBidder = msg.sender;
+        highestBid = msg.value;
+        emit HighestBidIncreased(msg.sender, msg.value);
+        if (previousHighestBidder != address(0)) {
+            (bool success, ) = previousHighestBidder.call{value: refundAmount}("");
+            require(success, "Failed to send back the ether!");
+        }
+        // ... other functions like auction end, withdrawal, etc.
+    }
+}
+</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>if (highestBidder != address(0)) {
+            (bool success, ) = highestBidder.call{value: highestBid}("");
+            require(success, "Failed to send back the ether!");
+        }
+        highestBidder = msg.sender;
+        highestBid = msg.value;</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>The vulnerability arises when calculating and distributing rewards. The contract updates user balance before updating the global interest rate, which means users can potentially claim more rewards than they should be able to.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">// SPDX-License-Identifier: MIT
+pragma solidity ^0.8.0;
+contract VulnerableRewardPool {
+    mapping(address =&gt; uint256) public balances;
+    uint256 public totalSupply;
+    uint256 public globalInterestRate = 1e18;
+    function deposit(uint256 amount) external {
+        // Update user balance
+        balances[msg.sender] += amount;
+        // Incorrect order: Updating global rate after user balance
+        updateGlobalInterestRate();
+        totalSupply += amount;
+    }
+    function claimRewards() external {
+        uint256 reward = balances[msg.sender] * globalInterestRate;
+        balances[msg.sender] += reward;
+        // Incorrect order: Updating global rate after user balance
+        updateGlobalInterestRate();
+    }
+    function updateGlobalInterestRate() internal {
+        // Assume some logic to increase global interest rate, e.g., 1% increment
+        globalInterestRate += globalInterestRate / 100;
+    }
+    // ... other functions
+}
+</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>balances[msg.sender] += amount;
+        // Incorrect order: Updating global rate after user balance
+        updateGlobalInterestRate();
+        totalSupply += amount;</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">// SPDX-License-Identifier: MIT
+pragma solidity ^0.8.0;
+contract SecureRewardPool {
+    mapping(address =&gt; uint256) public balances;
+    uint256 public totalSupply;
+    uint256 public globalInterestRate = 1e18;
+    function deposit(uint256 amount) external {
+        // Fix: Update global rate before user balance
+        updateGlobalInterestRate();
+        // Update user balance
+        balances[msg.sender] += amount;
+        totalSupply += amount;
+    }
+    function claimRewards() external {
+        // Fix: Update global rate before user balance
+        updateGlobalInterestRate();
+        uint256 reward = balances[msg.sender] * globalInterestRate;
+        balances[msg.sender] += reward;
+    }
+    function updateGlobalInterestRate() internal {
+        // Assume some logic to increase global interest rate, e.g., 1% increment
+        globalInterestRate += globalInterestRate / 100;
+    }
+    // ... other functions
+}
+</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Each deposit also earns a small interest for the user. However, the contract updates the user's principal deposit before applying the interest, leading to incorrect final balances.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">// SPDX-License-Identifier: MIT
+pragma solidity ^0.8.0;
+contract VulnerableLottery {
+    mapping(address =&gt; uint256) public balances;
+    uint256 public totalDeposits;
+    uint256 constant interestRate = 105; // 5% interest
+    function deposit(uint256 amount) external {
+        // Incorrect order: Updating the principal deposit before adding the interest
+        balances[msg.sender] += amount;
+        applyInterest(msg.sender);
+        totalDeposits += amount;
+    }
+    function applyInterest(address user) internal {
+        balances[user] = (balances[user] * interestRate) / 100;
+    }
+    // ... other functions like drawing a winner, etc.
+}
+</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve"> balances[msg.sender] += amount;
+        applyInterest(msg.sender);
+        totalDeposits += amount;</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">// SPDX-License-Identifier: MIT
+pragma solidity ^0.8.0;
+contract SecureLottery {
+    mapping(address =&gt; uint256) public balances;
+    uint256 public totalDeposits;
+    uint256 constant interestRate = 105; // 5% interest
+    function deposit(uint256 amount) external {
+        // Fix: Apply interest before updating the principal deposit
+        applyInterest(msg.sender);
+        balances[msg.sender] += amount;
+        totalDeposits += amount;
+    }
+    function applyInterest(address user) internal {
+        balances[user] = (balances[user] * interestRate) / 100;
+    }
+    // ... other functions like drawing a winner, etc.
+}
+</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>The contract offers a loyalty bonus to its users every time they deposit funds. However, the bonus is incorrectly added after updating the user's balance instead of before, leading to miscalculated total deposits.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">// SPDX-License-Identifier: MIT
+pragma solidity ^0.8.0;
+contract VulnerableBank {
+    mapping(address =&gt; uint256) public balances;
+    uint256 public totalDeposits;
+    uint256 constant loyaltyBonus = 10;  // 10 tokens bonus for each deposit
+    function deposit(uint256 amount) external {
+        balances[msg.sender] += amount;  // Incorrect order: updating balance before adding the bonus
+        giveLoyaltyBonus(msg.sender);
+        totalDeposits += amount;
+    }
+    function giveLoyaltyBonus(address user) internal {
+        balances[user] += loyaltyBonus;
+    }
+    // ... other functions like withdrawals, etc.
+}
+</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>balances[msg.sender] += amount;  // Incorrect order: updating balance before adding the bonus
+        giveLoyaltyBonus(msg.sender);
+        totalDeposits += amount;</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">// SPDX-License-Identifier: MIT
+pragma solidity ^0.8.0;
+contract FixedBank {
+    mapping(address =&gt; uint256) public balances;
+    uint256 public totalDeposits;
+    uint256 constant loyaltyBonus = 10;  // 10 tokens bonus for each deposit
+    function deposit(uint256 amount) external {
+        giveLoyaltyBonus(msg.sender);  // Fix: Add loyalty bonus before updating balance
+        balances[msg.sender] += amount;
+        totalDeposits += (amount + loyaltyBonus);  // Also consider the loyalty bonus in total deposits
+    }
+    function giveLoyaltyBonus(address user) internal {
+        balances[user] += loyaltyBonus;
+    }
+    // ... other functions like withdrawals, etc.
+}
+</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -12156,7 +12832,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -12181,11 +12857,21 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="20">
+  <dxfs count="21">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFF9900"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -12399,26 +13085,26 @@
     </dxf>
   </dxfs>
   <tableStyles count="2" defaultTableStyle="TableStylePreset3_Accent1" defaultPivotStyle="PivotStylePreset2_Accent1">
-    <tableStyle name="TableStylePreset3_Accent1" pivot="0" count="7" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
-      <tableStyleElement type="wholeTable" dxfId="19"/>
-      <tableStyleElement type="headerRow" dxfId="18"/>
-      <tableStyleElement type="totalRow" dxfId="17"/>
-      <tableStyleElement type="firstColumn" dxfId="16"/>
-      <tableStyleElement type="lastColumn" dxfId="15"/>
-      <tableStyleElement type="firstRowStripe" dxfId="14"/>
-      <tableStyleElement type="firstColumnStripe" dxfId="13"/>
+    <tableStyle name="TableStylePreset3_Accent1" pivot="0" count="7">
+      <tableStyleElement type="wholeTable" dxfId="20"/>
+      <tableStyleElement type="headerRow" dxfId="19"/>
+      <tableStyleElement type="totalRow" dxfId="18"/>
+      <tableStyleElement type="firstColumn" dxfId="17"/>
+      <tableStyleElement type="lastColumn" dxfId="16"/>
+      <tableStyleElement type="firstRowStripe" dxfId="15"/>
+      <tableStyleElement type="firstColumnStripe" dxfId="14"/>
     </tableStyle>
-    <tableStyle name="PivotStylePreset2_Accent1" table="0" count="10" xr9:uid="{00000000-0011-0000-FFFF-FFFF01000000}">
-      <tableStyleElement type="headerRow" dxfId="12"/>
-      <tableStyleElement type="totalRow" dxfId="11"/>
-      <tableStyleElement type="firstRowStripe" dxfId="10"/>
-      <tableStyleElement type="firstColumnStripe" dxfId="9"/>
-      <tableStyleElement type="firstSubtotalRow" dxfId="8"/>
-      <tableStyleElement type="secondSubtotalRow" dxfId="7"/>
-      <tableStyleElement type="firstRowSubheading" dxfId="6"/>
-      <tableStyleElement type="secondRowSubheading" dxfId="5"/>
-      <tableStyleElement type="pageFieldLabels" dxfId="4"/>
-      <tableStyleElement type="pageFieldValues" dxfId="3"/>
+    <tableStyle name="PivotStylePreset2_Accent1" table="0" count="10">
+      <tableStyleElement type="headerRow" dxfId="13"/>
+      <tableStyleElement type="totalRow" dxfId="12"/>
+      <tableStyleElement type="firstRowStripe" dxfId="11"/>
+      <tableStyleElement type="firstColumnStripe" dxfId="10"/>
+      <tableStyleElement type="firstSubtotalRow" dxfId="9"/>
+      <tableStyleElement type="secondSubtotalRow" dxfId="8"/>
+      <tableStyleElement type="firstRowSubheading" dxfId="7"/>
+      <tableStyleElement type="secondRowSubheading" dxfId="6"/>
+      <tableStyleElement type="pageFieldLabels" dxfId="5"/>
+      <tableStyleElement type="pageFieldValues" dxfId="4"/>
     </tableStyle>
   </tableStyles>
   <extLst>
@@ -12681,16 +13367,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E201"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E211"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A190" workbookViewId="0">
-      <selection activeCell="B201" sqref="B201"/>
+    <sheetView tabSelected="1" topLeftCell="A199" workbookViewId="0">
+      <selection activeCell="F210" sqref="F210"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>7</v>
       </c>
@@ -12707,7 +13393,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A2">
         <v>1</v>
       </c>
@@ -12724,7 +13410,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -12741,7 +13427,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -12758,7 +13444,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -12775,7 +13461,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -12792,7 +13478,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -12809,7 +13495,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -12826,7 +13512,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -12843,7 +13529,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -12860,7 +13546,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -12877,7 +13563,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -12894,7 +13580,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -12911,7 +13597,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -12928,7 +13614,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
@@ -12945,7 +13631,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
@@ -12962,7 +13648,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
@@ -12979,7 +13665,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
@@ -12996,7 +13682,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
@@ -13013,7 +13699,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
@@ -13030,7 +13716,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
@@ -13047,7 +13733,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
@@ -13064,7 +13750,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
@@ -13081,7 +13767,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
@@ -13098,7 +13784,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="25" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>24</v>
       </c>
@@ -13115,7 +13801,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="26" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>25</v>
       </c>
@@ -13132,7 +13818,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="27" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>26</v>
       </c>
@@ -13149,7 +13835,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="28" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>27</v>
       </c>
@@ -13166,7 +13852,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="29" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>28</v>
       </c>
@@ -13183,7 +13869,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="30" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>29</v>
       </c>
@@ -13200,7 +13886,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="31" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>30</v>
       </c>
@@ -13217,7 +13903,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="32" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>31</v>
       </c>
@@ -13234,7 +13920,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="33" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>32</v>
       </c>
@@ -13251,7 +13937,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="34" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>33</v>
       </c>
@@ -13268,7 +13954,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="35" spans="1:5" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:5" ht="16.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>34</v>
       </c>
@@ -13285,7 +13971,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="36" spans="1:5" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:5" ht="16.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>35</v>
       </c>
@@ -13302,7 +13988,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="37" spans="1:5" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:5" ht="16.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>36</v>
       </c>
@@ -13319,7 +14005,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="38" spans="1:5" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:5" ht="16.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>37</v>
       </c>
@@ -13336,7 +14022,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="39" spans="1:5" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:5" ht="16.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>38</v>
       </c>
@@ -13353,7 +14039,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="40" spans="1:5" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:5" ht="16.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>39</v>
       </c>
@@ -13370,7 +14056,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="41" spans="1:5" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:5" ht="16.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>40</v>
       </c>
@@ -13387,7 +14073,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="42" spans="1:5" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="42" spans="1:5" ht="16.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>41</v>
       </c>
@@ -13404,7 +14090,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="43" spans="1:5" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="43" spans="1:5" ht="16.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>42</v>
       </c>
@@ -13421,7 +14107,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="44" spans="1:5" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="44" spans="1:5" ht="16.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>43</v>
       </c>
@@ -13438,7 +14124,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="45" spans="1:5" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="45" spans="1:5" ht="16.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>44</v>
       </c>
@@ -13455,7 +14141,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="46" spans="1:5" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="46" spans="1:5" ht="16.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>45</v>
       </c>
@@ -13472,7 +14158,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="47" spans="1:5" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="47" spans="1:5" ht="16.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>46</v>
       </c>
@@ -13489,7 +14175,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="48" spans="1:5" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="48" spans="1:5" ht="16.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>47</v>
       </c>
@@ -13506,7 +14192,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="49" spans="1:5" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="49" spans="1:5" ht="16.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>48</v>
       </c>
@@ -13523,7 +14209,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="50" spans="1:5" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="50" spans="1:5" ht="16.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>49</v>
       </c>
@@ -13540,7 +14226,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="51" spans="1:5" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="51" spans="1:5" ht="16.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>50</v>
       </c>
@@ -13557,7 +14243,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="52" spans="1:5" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="52" spans="1:5" ht="16.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>51</v>
       </c>
@@ -13574,7 +14260,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="53" spans="1:5" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="53" spans="1:5" ht="16.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>52</v>
       </c>
@@ -13591,7 +14277,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="54" spans="1:5" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="54" spans="1:5" ht="16.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>53</v>
       </c>
@@ -13608,7 +14294,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="55" spans="1:5" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="55" spans="1:5" ht="16.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>54</v>
       </c>
@@ -13625,7 +14311,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="56" spans="1:5" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="56" spans="1:5" ht="16.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>55</v>
       </c>
@@ -13642,7 +14328,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="57" spans="1:5" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="57" spans="1:5" ht="16.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>56</v>
       </c>
@@ -13659,7 +14345,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="58" spans="1:5" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="58" spans="1:5" ht="16.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>57</v>
       </c>
@@ -13676,7 +14362,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="59" spans="1:5" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="59" spans="1:5" ht="16.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>58</v>
       </c>
@@ -13693,7 +14379,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="60" spans="1:5" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="60" spans="1:5" ht="16.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>59</v>
       </c>
@@ -13710,7 +14396,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="61" spans="1:5" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="61" spans="1:5" ht="16.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>60</v>
       </c>
@@ -13727,7 +14413,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="62" spans="1:5" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="62" spans="1:5" ht="16.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>61</v>
       </c>
@@ -13744,7 +14430,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="63" spans="1:5" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="63" spans="1:5" ht="16.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>62</v>
       </c>
@@ -13761,7 +14447,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="64" spans="1:5" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="64" spans="1:5" ht="16.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>63</v>
       </c>
@@ -13778,7 +14464,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="65" spans="1:5" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="65" spans="1:5" ht="16.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>64</v>
       </c>
@@ -13795,7 +14481,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="66" spans="1:5" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="66" spans="1:5" ht="16.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>65</v>
       </c>
@@ -13812,7 +14498,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="67" spans="1:5" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="67" spans="1:5" ht="16.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>66</v>
       </c>
@@ -13829,7 +14515,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="68" spans="1:5" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="68" spans="1:5" ht="16.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>67</v>
       </c>
@@ -13846,7 +14532,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="69" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="69" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>68</v>
       </c>
@@ -13863,7 +14549,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="70" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="70" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>69</v>
       </c>
@@ -13880,7 +14566,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="71" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="71" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>70</v>
       </c>
@@ -13897,7 +14583,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="72" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="72" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>71</v>
       </c>
@@ -13914,7 +14600,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="73" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="73" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>72</v>
       </c>
@@ -13931,7 +14617,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="74" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="74" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>73</v>
       </c>
@@ -13948,7 +14634,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="75" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="75" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>74</v>
       </c>
@@ -13965,7 +14651,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="76" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="76" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>75</v>
       </c>
@@ -13982,7 +14668,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="77" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="77" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>76</v>
       </c>
@@ -13999,7 +14685,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="78" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="78" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>77</v>
       </c>
@@ -14016,7 +14702,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="79" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="79" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>78</v>
       </c>
@@ -14033,7 +14719,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="80" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="80" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>79</v>
       </c>
@@ -14050,7 +14736,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="81" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="81" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>80</v>
       </c>
@@ -14067,7 +14753,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="82" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="82" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>81</v>
       </c>
@@ -14084,7 +14770,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="83" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="83" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>82</v>
       </c>
@@ -14101,7 +14787,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="84" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="84" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>83</v>
       </c>
@@ -14118,7 +14804,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="85" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="85" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>84</v>
       </c>
@@ -14135,7 +14821,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="86" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="86" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>85</v>
       </c>
@@ -14152,7 +14838,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="87" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="87" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>86</v>
       </c>
@@ -14169,7 +14855,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="88" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="88" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>87</v>
       </c>
@@ -14186,7 +14872,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="89" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="89" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>88</v>
       </c>
@@ -14203,7 +14889,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="90" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="90" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>89</v>
       </c>
@@ -14220,7 +14906,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="91" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="91" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>90</v>
       </c>
@@ -14237,7 +14923,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="92" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="92" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A92">
         <v>91</v>
       </c>
@@ -14254,7 +14940,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="93" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="93" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A93">
         <v>92</v>
       </c>
@@ -14271,7 +14957,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="94" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="94" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A94">
         <v>93</v>
       </c>
@@ -14288,7 +14974,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="95" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="95" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A95">
         <v>94</v>
       </c>
@@ -14305,7 +14991,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="96" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="96" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A96">
         <v>95</v>
       </c>
@@ -14322,7 +15008,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="97" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="97" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A97">
         <v>96</v>
       </c>
@@ -14339,7 +15025,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="98" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="98" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A98">
         <v>97</v>
       </c>
@@ -14356,7 +15042,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="99" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="99" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A99">
         <v>98</v>
       </c>
@@ -14373,7 +15059,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="100" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="100" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A100">
         <v>99</v>
       </c>
@@ -14390,7 +15076,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="101" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="101" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A101">
         <v>100</v>
       </c>
@@ -14407,7 +15093,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="102" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="102" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A102">
         <v>101</v>
       </c>
@@ -14424,7 +15110,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="103" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="103" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A103">
         <v>102</v>
       </c>
@@ -14441,7 +15127,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="104" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="104" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A104">
         <v>103</v>
       </c>
@@ -14458,7 +15144,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="105" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="105" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A105">
         <v>104</v>
       </c>
@@ -14475,7 +15161,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="106" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="106" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A106">
         <v>105</v>
       </c>
@@ -14492,7 +15178,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="107" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="107" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A107">
         <v>106</v>
       </c>
@@ -14509,7 +15195,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="108" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="108" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A108">
         <v>107</v>
       </c>
@@ -14526,7 +15212,7 @@
         <v>418</v>
       </c>
     </row>
-    <row r="109" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="109" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A109">
         <v>108</v>
       </c>
@@ -14543,7 +15229,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="110" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="110" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A110">
         <v>109</v>
       </c>
@@ -14560,7 +15246,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="111" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="111" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A111">
         <v>110</v>
       </c>
@@ -14577,7 +15263,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="112" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="112" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A112">
         <v>111</v>
       </c>
@@ -14594,7 +15280,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="113" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="113" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A113">
         <v>112</v>
       </c>
@@ -14611,7 +15297,7 @@
         <v>438</v>
       </c>
     </row>
-    <row r="114" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="114" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A114">
         <v>113</v>
       </c>
@@ -14628,7 +15314,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="115" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="115" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A115">
         <v>114</v>
       </c>
@@ -14645,7 +15331,7 @@
         <v>444</v>
       </c>
     </row>
-    <row r="116" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="116" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A116">
         <v>115</v>
       </c>
@@ -14662,7 +15348,7 @@
         <v>448</v>
       </c>
     </row>
-    <row r="117" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="117" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A117">
         <v>116</v>
       </c>
@@ -14679,7 +15365,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="118" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="118" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A118">
         <v>117</v>
       </c>
@@ -14696,7 +15382,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="119" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="119" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A119">
         <v>118</v>
       </c>
@@ -14713,7 +15399,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="120" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="120" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A120">
         <v>119</v>
       </c>
@@ -14730,7 +15416,7 @@
         <v>462</v>
       </c>
     </row>
-    <row r="121" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="121" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A121">
         <v>120</v>
       </c>
@@ -14747,7 +15433,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="122" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="122" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A122">
         <v>121</v>
       </c>
@@ -14764,7 +15450,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="123" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="123" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A123">
         <v>122</v>
       </c>
@@ -14781,7 +15467,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="124" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="124" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A124">
         <v>123</v>
       </c>
@@ -14798,7 +15484,7 @@
         <v>477</v>
       </c>
     </row>
-    <row r="125" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="125" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A125">
         <v>124</v>
       </c>
@@ -14815,7 +15501,7 @@
         <v>499</v>
       </c>
     </row>
-    <row r="126" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="126" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A126">
         <v>125</v>
       </c>
@@ -14832,7 +15518,7 @@
         <v>503</v>
       </c>
     </row>
-    <row r="127" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="127" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A127">
         <v>126</v>
       </c>
@@ -14849,7 +15535,7 @@
         <v>507</v>
       </c>
     </row>
-    <row r="128" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="128" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A128">
         <v>127</v>
       </c>
@@ -14866,7 +15552,7 @@
         <v>511</v>
       </c>
     </row>
-    <row r="129" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="129" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A129">
         <v>128</v>
       </c>
@@ -14883,7 +15569,7 @@
         <v>515</v>
       </c>
     </row>
-    <row r="130" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="130" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A130">
         <v>129</v>
       </c>
@@ -14900,7 +15586,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="131" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="131" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A131">
         <v>130</v>
       </c>
@@ -14917,7 +15603,7 @@
         <v>523</v>
       </c>
     </row>
-    <row r="132" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="132" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A132">
         <v>131</v>
       </c>
@@ -14934,7 +15620,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="133" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="133" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A133">
         <v>132</v>
       </c>
@@ -14951,7 +15637,7 @@
         <v>531</v>
       </c>
     </row>
-    <row r="134" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="134" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A134">
         <v>133</v>
       </c>
@@ -14968,7 +15654,7 @@
         <v>536</v>
       </c>
     </row>
-    <row r="135" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="135" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A135">
         <v>134</v>
       </c>
@@ -14985,7 +15671,7 @@
         <v>540</v>
       </c>
     </row>
-    <row r="136" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="136" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A136">
         <v>135</v>
       </c>
@@ -15019,7 +15705,7 @@
         <v>548</v>
       </c>
     </row>
-    <row r="138" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="138" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A138">
         <v>137</v>
       </c>
@@ -15036,7 +15722,7 @@
         <v>552</v>
       </c>
     </row>
-    <row r="139" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="139" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A139">
         <v>138</v>
       </c>
@@ -15053,7 +15739,7 @@
         <v>556</v>
       </c>
     </row>
-    <row r="140" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="140" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A140">
         <v>139</v>
       </c>
@@ -15070,7 +15756,7 @@
         <v>560</v>
       </c>
     </row>
-    <row r="141" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="141" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A141">
         <v>140</v>
       </c>
@@ -15087,7 +15773,7 @@
         <v>564</v>
       </c>
     </row>
-    <row r="142" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="142" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A142">
         <v>141</v>
       </c>
@@ -15104,7 +15790,7 @@
         <v>568</v>
       </c>
     </row>
-    <row r="143" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="143" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A143">
         <v>142</v>
       </c>
@@ -15121,7 +15807,7 @@
         <v>572</v>
       </c>
     </row>
-    <row r="144" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="144" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A144">
         <v>143</v>
       </c>
@@ -15138,7 +15824,7 @@
         <v>576</v>
       </c>
     </row>
-    <row r="145" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="145" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A145">
         <v>144</v>
       </c>
@@ -15155,7 +15841,7 @@
         <v>579</v>
       </c>
     </row>
-    <row r="146" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="146" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A146">
         <v>145</v>
       </c>
@@ -15172,7 +15858,7 @@
         <v>583</v>
       </c>
     </row>
-    <row r="147" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="147" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A147">
         <v>146</v>
       </c>
@@ -15189,7 +15875,7 @@
         <v>587</v>
       </c>
     </row>
-    <row r="148" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="148" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A148">
         <v>147</v>
       </c>
@@ -15206,7 +15892,7 @@
         <v>591</v>
       </c>
     </row>
-    <row r="149" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="149" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A149">
         <v>148</v>
       </c>
@@ -15223,7 +15909,7 @@
         <v>595</v>
       </c>
     </row>
-    <row r="150" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="150" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A150">
         <v>149</v>
       </c>
@@ -15240,7 +15926,7 @@
         <v>599</v>
       </c>
     </row>
-    <row r="151" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="151" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A151">
         <v>150</v>
       </c>
@@ -15257,7 +15943,7 @@
         <v>603</v>
       </c>
     </row>
-    <row r="152" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="152" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A152">
         <v>151</v>
       </c>
@@ -15274,7 +15960,7 @@
         <v>607</v>
       </c>
     </row>
-    <row r="153" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="153" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A153">
         <v>152</v>
       </c>
@@ -15291,7 +15977,7 @@
         <v>611</v>
       </c>
     </row>
-    <row r="154" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="154" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A154">
         <v>153</v>
       </c>
@@ -15308,7 +15994,7 @@
         <v>615</v>
       </c>
     </row>
-    <row r="155" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="155" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A155">
         <v>154</v>
       </c>
@@ -15325,7 +16011,7 @@
         <v>619</v>
       </c>
     </row>
-    <row r="156" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="156" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A156">
         <v>155</v>
       </c>
@@ -15342,7 +16028,7 @@
         <v>623</v>
       </c>
     </row>
-    <row r="157" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="157" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A157">
         <v>156</v>
       </c>
@@ -15359,7 +16045,7 @@
         <v>627</v>
       </c>
     </row>
-    <row r="158" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="158" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A158">
         <v>157</v>
       </c>
@@ -15376,7 +16062,7 @@
         <v>631</v>
       </c>
     </row>
-    <row r="159" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="159" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A159">
         <v>158</v>
       </c>
@@ -15393,7 +16079,7 @@
         <v>635</v>
       </c>
     </row>
-    <row r="160" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="160" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A160">
         <v>159</v>
       </c>
@@ -15410,7 +16096,7 @@
         <v>639</v>
       </c>
     </row>
-    <row r="161" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="161" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A161">
         <v>160</v>
       </c>
@@ -15427,7 +16113,7 @@
         <v>643</v>
       </c>
     </row>
-    <row r="162" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="162" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A162">
         <v>161</v>
       </c>
@@ -15444,7 +16130,7 @@
         <v>647</v>
       </c>
     </row>
-    <row r="163" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="163" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A163">
         <v>162</v>
       </c>
@@ -15461,7 +16147,7 @@
         <v>651</v>
       </c>
     </row>
-    <row r="164" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="164" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A164">
         <v>163</v>
       </c>
@@ -15478,7 +16164,7 @@
         <v>655</v>
       </c>
     </row>
-    <row r="165" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="165" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A165">
         <v>164</v>
       </c>
@@ -15495,7 +16181,7 @@
         <v>659</v>
       </c>
     </row>
-    <row r="166" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="166" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A166">
         <v>165</v>
       </c>
@@ -15512,7 +16198,7 @@
         <v>663</v>
       </c>
     </row>
-    <row r="167" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="167" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A167">
         <v>166</v>
       </c>
@@ -15529,7 +16215,7 @@
         <v>667</v>
       </c>
     </row>
-    <row r="168" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="168" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A168">
         <v>167</v>
       </c>
@@ -15546,7 +16232,7 @@
         <v>671</v>
       </c>
     </row>
-    <row r="169" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="169" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A169">
         <v>168</v>
       </c>
@@ -15563,7 +16249,7 @@
         <v>675</v>
       </c>
     </row>
-    <row r="170" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="170" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A170">
         <v>169</v>
       </c>
@@ -15580,7 +16266,7 @@
         <v>679</v>
       </c>
     </row>
-    <row r="171" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="171" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A171">
         <v>170</v>
       </c>
@@ -15597,7 +16283,7 @@
         <v>683</v>
       </c>
     </row>
-    <row r="172" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="172" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A172">
         <v>171</v>
       </c>
@@ -15614,7 +16300,7 @@
         <v>687</v>
       </c>
     </row>
-    <row r="173" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="173" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A173">
         <v>172</v>
       </c>
@@ -15631,7 +16317,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="174" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="174" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A174">
         <v>173</v>
       </c>
@@ -15648,7 +16334,7 @@
         <v>695</v>
       </c>
     </row>
-    <row r="175" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="175" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A175">
         <v>174</v>
       </c>
@@ -15665,7 +16351,7 @@
         <v>699</v>
       </c>
     </row>
-    <row r="176" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="176" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A176">
         <v>175</v>
       </c>
@@ -15682,7 +16368,7 @@
         <v>703</v>
       </c>
     </row>
-    <row r="177" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="177" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A177">
         <v>176</v>
       </c>
@@ -15699,7 +16385,7 @@
         <v>707</v>
       </c>
     </row>
-    <row r="178" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="178" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A178">
         <v>177</v>
       </c>
@@ -15716,7 +16402,7 @@
         <v>711</v>
       </c>
     </row>
-    <row r="179" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="179" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A179">
         <v>178</v>
       </c>
@@ -15733,7 +16419,7 @@
         <v>715</v>
       </c>
     </row>
-    <row r="180" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="180" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A180">
         <v>179</v>
       </c>
@@ -15750,7 +16436,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="181" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="181" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A181">
         <v>180</v>
       </c>
@@ -15767,7 +16453,7 @@
         <v>723</v>
       </c>
     </row>
-    <row r="182" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="182" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A182">
         <v>181</v>
       </c>
@@ -15784,7 +16470,7 @@
         <v>727</v>
       </c>
     </row>
-    <row r="183" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="183" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A183">
         <v>182</v>
       </c>
@@ -15801,7 +16487,7 @@
         <v>731</v>
       </c>
     </row>
-    <row r="184" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="184" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A184">
         <v>183</v>
       </c>
@@ -15818,7 +16504,7 @@
         <v>735</v>
       </c>
     </row>
-    <row r="185" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="185" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A185">
         <v>184</v>
       </c>
@@ -15835,7 +16521,7 @@
         <v>739</v>
       </c>
     </row>
-    <row r="186" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="186" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A186">
         <v>185</v>
       </c>
@@ -15852,7 +16538,7 @@
         <v>742</v>
       </c>
     </row>
-    <row r="187" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="187" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A187">
         <v>186</v>
       </c>
@@ -15869,7 +16555,7 @@
         <v>746</v>
       </c>
     </row>
-    <row r="188" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="188" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A188">
         <v>187</v>
       </c>
@@ -15886,7 +16572,7 @@
         <v>750</v>
       </c>
     </row>
-    <row r="189" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="189" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A189">
         <v>188</v>
       </c>
@@ -15903,7 +16589,7 @@
         <v>754</v>
       </c>
     </row>
-    <row r="190" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="190" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A190">
         <v>189</v>
       </c>
@@ -15920,7 +16606,7 @@
         <v>758</v>
       </c>
     </row>
-    <row r="191" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="191" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A191">
         <v>190</v>
       </c>
@@ -15937,7 +16623,7 @@
         <v>762</v>
       </c>
     </row>
-    <row r="192" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="192" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A192">
         <v>191</v>
       </c>
@@ -15954,7 +16640,7 @@
         <v>766</v>
       </c>
     </row>
-    <row r="193" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="193" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A193">
         <v>192</v>
       </c>
@@ -15971,7 +16657,7 @@
         <v>770</v>
       </c>
     </row>
-    <row r="194" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="194" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A194">
         <v>193</v>
       </c>
@@ -15988,7 +16674,7 @@
         <v>774</v>
       </c>
     </row>
-    <row r="195" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="195" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A195">
         <v>194</v>
       </c>
@@ -16005,7 +16691,7 @@
         <v>778</v>
       </c>
     </row>
-    <row r="196" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="196" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A196">
         <v>195</v>
       </c>
@@ -16022,7 +16708,7 @@
         <v>782</v>
       </c>
     </row>
-    <row r="197" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="197" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A197">
         <v>196</v>
       </c>
@@ -16039,7 +16725,7 @@
         <v>786</v>
       </c>
     </row>
-    <row r="198" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="198" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A198">
         <v>197</v>
       </c>
@@ -16056,7 +16742,7 @@
         <v>790</v>
       </c>
     </row>
-    <row r="199" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="199" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A199">
         <v>198</v>
       </c>
@@ -16073,7 +16759,7 @@
         <v>794</v>
       </c>
     </row>
-    <row r="200" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="200" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A200">
         <v>199</v>
       </c>
@@ -16090,7 +16776,7 @@
         <v>798</v>
       </c>
     </row>
-    <row r="201" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="201" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A201">
         <v>200</v>
       </c>
@@ -16105,19 +16791,193 @@
       </c>
       <c r="E201" s="2" t="s">
         <v>802</v>
+      </c>
+    </row>
+    <row r="202" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A202">
+        <v>201</v>
+      </c>
+      <c r="B202" s="2" t="s">
+        <v>803</v>
+      </c>
+      <c r="C202" s="2" t="s">
+        <v>804</v>
+      </c>
+      <c r="D202" s="7" t="s">
+        <v>805</v>
+      </c>
+      <c r="E202" s="12" t="s">
+        <v>807</v>
+      </c>
+    </row>
+    <row r="203" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A203">
+        <v>202</v>
+      </c>
+      <c r="B203" s="7" t="s">
+        <v>808</v>
+      </c>
+      <c r="C203" s="7" t="s">
+        <v>809</v>
+      </c>
+      <c r="D203" s="7" t="s">
+        <v>810</v>
+      </c>
+      <c r="E203" s="12" t="s">
+        <v>806</v>
+      </c>
+    </row>
+    <row r="204" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A204">
+        <v>203</v>
+      </c>
+      <c r="B204" s="7" t="s">
+        <v>812</v>
+      </c>
+      <c r="C204" s="7" t="s">
+        <v>814</v>
+      </c>
+      <c r="D204" s="7" t="s">
+        <v>813</v>
+      </c>
+      <c r="E204" s="12" t="s">
+        <v>811</v>
+      </c>
+    </row>
+    <row r="205" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A205">
+        <v>204</v>
+      </c>
+      <c r="B205" s="7" t="s">
+        <v>816</v>
+      </c>
+      <c r="C205" s="7" t="s">
+        <v>817</v>
+      </c>
+      <c r="D205" s="7" t="s">
+        <v>818</v>
+      </c>
+      <c r="E205" s="12" t="s">
+        <v>815</v>
+      </c>
+    </row>
+    <row r="206" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A206">
+        <v>205</v>
+      </c>
+      <c r="B206" s="7" t="s">
+        <v>820</v>
+      </c>
+      <c r="C206" s="7" t="s">
+        <v>822</v>
+      </c>
+      <c r="D206" s="7" t="s">
+        <v>821</v>
+      </c>
+      <c r="E206" s="12" t="s">
+        <v>819</v>
+      </c>
+    </row>
+    <row r="207" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A207">
+        <v>206</v>
+      </c>
+      <c r="B207" s="7" t="s">
+        <v>824</v>
+      </c>
+      <c r="C207" s="7" t="s">
+        <v>826</v>
+      </c>
+      <c r="D207" s="7" t="s">
+        <v>825</v>
+      </c>
+      <c r="E207" s="12" t="s">
+        <v>823</v>
+      </c>
+    </row>
+    <row r="208" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A208">
+        <v>207</v>
+      </c>
+      <c r="B208" s="7" t="s">
+        <v>828</v>
+      </c>
+      <c r="C208" s="7" t="s">
+        <v>829</v>
+      </c>
+      <c r="D208" s="7" t="s">
+        <v>830</v>
+      </c>
+      <c r="E208" s="12" t="s">
+        <v>827</v>
+      </c>
+    </row>
+    <row r="209" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A209">
+        <v>208</v>
+      </c>
+      <c r="B209" s="7" t="s">
+        <v>832</v>
+      </c>
+      <c r="C209" s="7" t="s">
+        <v>834</v>
+      </c>
+      <c r="D209" s="7" t="s">
+        <v>833</v>
+      </c>
+      <c r="E209" s="12" t="s">
+        <v>831</v>
+      </c>
+    </row>
+    <row r="210" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A210">
+        <v>209</v>
+      </c>
+      <c r="B210" s="7" t="s">
+        <v>836</v>
+      </c>
+      <c r="C210" s="7" t="s">
+        <v>838</v>
+      </c>
+      <c r="D210" s="7" t="s">
+        <v>837</v>
+      </c>
+      <c r="E210" s="12" t="s">
+        <v>835</v>
+      </c>
+    </row>
+    <row r="211" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A211">
+        <v>210</v>
+      </c>
+      <c r="B211" s="7" t="s">
+        <v>840</v>
+      </c>
+      <c r="C211" s="7" t="s">
+        <v>842</v>
+      </c>
+      <c r="D211" s="7" t="s">
+        <v>841</v>
+      </c>
+      <c r="E211" s="12" t="s">
+        <v>839</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="B80:C82 B35:E78 D80:E93 B95:E103 B105:E106 B108:E122 B124:E124 B84:C93">
+    <cfRule type="duplicateValues" dxfId="3" priority="4"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B83:C83">
     <cfRule type="duplicateValues" dxfId="2" priority="3"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B83:C83">
+  <conditionalFormatting sqref="B192:E201 E203:E211">
     <cfRule type="duplicateValues" dxfId="1" priority="2"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B192:E201">
+  <conditionalFormatting sqref="E202">
     <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>